<commit_message>
added functions for text fragmenting
</commit_message>
<xml_diff>
--- a/admin/Schedule of Activity.xlsx
+++ b/admin/Schedule of Activity.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b94ccae29788f3bc/Bristol/Final Year Project/w5/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C21C6F58-1014-4864-8FB2-26715C64A931}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{83333B75-0E7F-478E-A0AE-387AA93C5A21}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="4020" xr2:uid="{BC5E3FEA-07E1-42A4-AA4A-5DAF8469F5C2}"/>
   </bookViews>
@@ -671,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41896FE7-47FE-4192-B182-9F96C4005BA7}">
   <dimension ref="A1:P1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0" xr3:uid="{D07F2CD1-9907-54B6-B695-3108A5814274}">
-      <selection activeCell="J16" sqref="J8:Q16"/>
+    <sheetView tabSelected="1" zoomScale="83" zoomScaleNormal="83" workbookViewId="0" xr3:uid="{D07F2CD1-9907-54B6-B695-3108A5814274}">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45"/>
@@ -1112,15 +1112,19 @@
       <c r="E11" t="s">
         <v>26</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="F11" s="1">
+        <v>43413</v>
+      </c>
+      <c r="G11" s="1">
+        <v>43413</v>
+      </c>
       <c r="H11" s="7" t="str">
         <f>IF(NOT(Table3[End_]=""),L11,"")</f>
-        <v/>
+        <v>YES</v>
       </c>
       <c r="I11" s="7" t="str">
         <f>IF(NOT(Table3[End_]=""),M11,"")</f>
-        <v/>
+        <v>YES</v>
       </c>
       <c r="L11" s="5" t="str">
         <f t="shared" si="0"/>
@@ -1155,15 +1159,19 @@
       <c r="E12" t="s">
         <v>26</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="F12" s="1">
+        <v>43413</v>
+      </c>
+      <c r="G12" s="1">
+        <v>43413</v>
+      </c>
       <c r="H12" s="7" t="str">
         <f>IF(NOT(Table3[End_]=""),L12,"")</f>
-        <v/>
+        <v>YES</v>
       </c>
       <c r="I12" s="7" t="str">
         <f>IF(NOT(Table3[End_]=""),M12,"")</f>
-        <v/>
+        <v>YES</v>
       </c>
       <c r="L12" s="5" t="str">
         <f t="shared" si="0"/>

</xml_diff>